<commit_message>
03Mar2020-Fixes 1. PURCHASE ORDER – FOUR DECIMAL PLACE - Done 2. SEARCH BAR – Done 3. INVENTORY IS MISSING PONO 83468 – Done b. FOR VALIDATED SO AND LATER CANCELLED – Done
</commit_message>
<xml_diff>
--- a/Solution.FC2J/MasterData/PurchaseOrder-POHeaderID10.xlsx
+++ b/Solution.FC2J/MasterData/PurchaseOrder-POHeaderID10.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\source\repos\ProjectYuan-WMS\Solution.FC2J\MasterData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C7E3363F-3584-479A-BAD4-C6775B52852C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAA134A7-4127-4551-BFE6-48651917426A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{9231E1FA-3742-412A-98F3-FAAC9C358490}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="92">
   <si>
     <t>SUB TOTAL</t>
   </si>
@@ -310,14 +310,18 @@
   </si>
   <si>
     <t xml:space="preserve">AND POHeaderId = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDATE [sale.order.detail].FC2J SET TaxPrice = </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -374,7 +378,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -385,6 +389,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -752,7 +758,7 @@
   <dimension ref="A1:AW35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:F13"/>
+      <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2178,21 +2184,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{932AA0DA-EFCE-4A8A-98DC-948ACD101D99}">
-  <dimension ref="E5:K17"/>
+  <dimension ref="E5:L25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6:K17"/>
+      <selection activeCell="F22" sqref="F22:K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="45" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="45" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E5" t="s">
         <v>5</v>
       </c>
@@ -2203,7 +2211,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E6">
         <v>1</v>
       </c>
@@ -2227,7 +2235,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E7">
         <v>2</v>
       </c>
@@ -2251,7 +2259,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E8">
         <v>3</v>
       </c>
@@ -2275,7 +2283,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E9">
         <v>4</v>
       </c>
@@ -2299,7 +2307,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E10">
         <v>5</v>
       </c>
@@ -2323,7 +2331,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E11">
         <v>6</v>
       </c>
@@ -2347,7 +2355,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E12">
         <v>7</v>
       </c>
@@ -2371,7 +2379,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E13" s="8">
         <v>8</v>
       </c>
@@ -2395,7 +2403,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E14" s="7">
         <v>9</v>
       </c>
@@ -2418,8 +2426,11 @@
       <c r="K14" s="7">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L14" s="10">
+        <v>14909.348160000001</v>
+      </c>
+    </row>
+    <row r="15" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E15" s="7">
         <v>10</v>
       </c>
@@ -2442,8 +2453,11 @@
       <c r="K15" s="7">
         <v>10</v>
       </c>
-    </row>
-    <row r="16" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L15" s="10">
+        <v>14863.375485</v>
+      </c>
+    </row>
+    <row r="16" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E16" s="7">
         <v>11</v>
       </c>
@@ -2466,8 +2480,11 @@
       <c r="K16" s="7">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L16" s="10">
+        <v>3865.3889400000003</v>
+      </c>
+    </row>
+    <row r="17" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E17" s="7">
         <v>12</v>
       </c>
@@ -2488,6 +2505,94 @@
         <v>90</v>
       </c>
       <c r="K17" s="7">
+        <v>10</v>
+      </c>
+      <c r="L17">
+        <v>2024.7255</v>
+      </c>
+    </row>
+    <row r="20" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="F22" t="s">
+        <v>91</v>
+      </c>
+      <c r="G22" s="10">
+        <v>14909.348160000001</v>
+      </c>
+      <c r="H22" t="s">
+        <v>89</v>
+      </c>
+      <c r="I22" s="7">
+        <v>20108</v>
+      </c>
+      <c r="J22" t="s">
+        <v>90</v>
+      </c>
+      <c r="K22" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="F23" t="s">
+        <v>91</v>
+      </c>
+      <c r="G23" s="10">
+        <v>14863.375485</v>
+      </c>
+      <c r="H23" t="s">
+        <v>89</v>
+      </c>
+      <c r="I23" s="7">
+        <v>20109</v>
+      </c>
+      <c r="J23" t="s">
+        <v>90</v>
+      </c>
+      <c r="K23" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="F24" t="s">
+        <v>91</v>
+      </c>
+      <c r="G24" s="10">
+        <v>3865.3889400000003</v>
+      </c>
+      <c r="H24" t="s">
+        <v>89</v>
+      </c>
+      <c r="I24" s="7">
+        <v>20110</v>
+      </c>
+      <c r="J24" t="s">
+        <v>90</v>
+      </c>
+      <c r="K24" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="F25" t="s">
+        <v>91</v>
+      </c>
+      <c r="G25">
+        <v>2024.7255</v>
+      </c>
+      <c r="H25" t="s">
+        <v>89</v>
+      </c>
+      <c r="I25" s="7">
+        <v>20111</v>
+      </c>
+      <c r="J25" t="s">
+        <v>90</v>
+      </c>
+      <c r="K25" s="7">
         <v>10</v>
       </c>
     </row>
@@ -2498,10 +2603,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05A5A94D-55A3-4EA8-B666-11E8EB7039E3}">
-  <dimension ref="A1:T16"/>
+  <dimension ref="A1:U38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2520,14 +2625,15 @@
     <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -2573,23 +2679,23 @@
       <c r="O1" t="s">
         <v>17</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>18</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>19</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>20</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>21</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>89</v>
       </c>
@@ -2635,23 +2741,23 @@
       <c r="O2">
         <v>0</v>
       </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
       <c r="Q2">
         <v>0</v>
       </c>
-      <c r="R2" t="s">
-        <v>27</v>
+      <c r="R2">
+        <v>0</v>
       </c>
       <c r="S2" t="s">
         <v>27</v>
       </c>
-      <c r="T2">
+      <c r="T2" t="s">
+        <v>27</v>
+      </c>
+      <c r="U2">
         <v>12345</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>90</v>
       </c>
@@ -2697,23 +2803,23 @@
       <c r="O3">
         <v>0</v>
       </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
       <c r="Q3">
         <v>0</v>
       </c>
-      <c r="R3" t="s">
-        <v>27</v>
+      <c r="R3">
+        <v>0</v>
       </c>
       <c r="S3" t="s">
         <v>27</v>
       </c>
-      <c r="T3">
+      <c r="T3" t="s">
+        <v>27</v>
+      </c>
+      <c r="U3">
         <v>12345</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>91</v>
       </c>
@@ -2759,23 +2865,23 @@
       <c r="O4">
         <v>0</v>
       </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
       <c r="Q4">
         <v>0</v>
       </c>
-      <c r="R4" t="s">
-        <v>27</v>
+      <c r="R4">
+        <v>0</v>
       </c>
       <c r="S4" t="s">
         <v>27</v>
       </c>
-      <c r="T4">
+      <c r="T4" t="s">
+        <v>27</v>
+      </c>
+      <c r="U4">
         <v>12344</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>92</v>
       </c>
@@ -2821,23 +2927,23 @@
       <c r="O5">
         <v>0</v>
       </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
       <c r="Q5">
         <v>0</v>
       </c>
-      <c r="R5" t="s">
-        <v>27</v>
+      <c r="R5">
+        <v>0</v>
       </c>
       <c r="S5" t="s">
         <v>27</v>
       </c>
-      <c r="T5">
+      <c r="T5" t="s">
+        <v>27</v>
+      </c>
+      <c r="U5">
         <v>12344</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>93</v>
       </c>
@@ -2883,23 +2989,23 @@
       <c r="O6">
         <v>0</v>
       </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
       <c r="Q6">
         <v>0</v>
       </c>
-      <c r="R6" t="s">
-        <v>27</v>
+      <c r="R6">
+        <v>0</v>
       </c>
       <c r="S6" t="s">
         <v>27</v>
       </c>
-      <c r="T6">
+      <c r="T6" t="s">
+        <v>27</v>
+      </c>
+      <c r="U6">
         <v>12343</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>94</v>
       </c>
@@ -2945,23 +3051,23 @@
       <c r="O7">
         <v>0</v>
       </c>
-      <c r="P7">
-        <v>0</v>
-      </c>
       <c r="Q7">
         <v>0</v>
       </c>
-      <c r="R7" t="s">
-        <v>27</v>
+      <c r="R7">
+        <v>0</v>
       </c>
       <c r="S7" t="s">
         <v>27</v>
       </c>
-      <c r="T7">
+      <c r="T7" t="s">
+        <v>27</v>
+      </c>
+      <c r="U7">
         <v>12343</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>95</v>
       </c>
@@ -3007,23 +3113,23 @@
       <c r="O8">
         <v>0</v>
       </c>
-      <c r="P8">
-        <v>0</v>
-      </c>
       <c r="Q8">
         <v>0</v>
       </c>
-      <c r="R8" t="s">
-        <v>27</v>
+      <c r="R8">
+        <v>0</v>
       </c>
       <c r="S8" t="s">
         <v>27</v>
       </c>
-      <c r="T8">
+      <c r="T8" t="s">
+        <v>27</v>
+      </c>
+      <c r="U8">
         <v>12343</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>96</v>
       </c>
@@ -3069,23 +3175,23 @@
       <c r="O9">
         <v>0</v>
       </c>
-      <c r="P9">
-        <v>0</v>
-      </c>
       <c r="Q9">
         <v>0</v>
       </c>
-      <c r="R9" t="s">
-        <v>27</v>
+      <c r="R9">
+        <v>0</v>
       </c>
       <c r="S9" t="s">
         <v>27</v>
       </c>
-      <c r="T9">
+      <c r="T9" t="s">
+        <v>27</v>
+      </c>
+      <c r="U9">
         <v>12343</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>97</v>
       </c>
@@ -3131,20 +3237,24 @@
       <c r="O10">
         <v>0.1071</v>
       </c>
-      <c r="P10">
+      <c r="P10" s="10">
+        <f>M10*O10</f>
+        <v>14909.348160000001</v>
+      </c>
+      <c r="Q10">
         <v>14915.3143</v>
       </c>
-      <c r="Q10">
-        <v>0</v>
-      </c>
-      <c r="R10" t="s">
-        <v>27</v>
+      <c r="R10">
+        <v>0</v>
       </c>
       <c r="S10" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>98</v>
       </c>
@@ -3190,20 +3300,24 @@
       <c r="O11">
         <v>0.1071</v>
       </c>
-      <c r="P11">
+      <c r="P11" s="10">
+        <f t="shared" ref="P11:P13" si="0">M11*O11</f>
+        <v>14863.375485</v>
+      </c>
+      <c r="Q11">
         <v>14869.323200000001</v>
       </c>
-      <c r="Q11">
-        <v>0</v>
-      </c>
-      <c r="R11" t="s">
-        <v>27</v>
+      <c r="R11">
+        <v>0</v>
       </c>
       <c r="S11" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>99</v>
       </c>
@@ -3249,20 +3363,24 @@
       <c r="O12">
         <v>0.1071</v>
       </c>
-      <c r="P12">
+      <c r="P12" s="10">
+        <f t="shared" si="0"/>
+        <v>3865.3889400000003</v>
+      </c>
+      <c r="Q12">
         <v>3866.9357</v>
       </c>
-      <c r="Q12">
-        <v>0</v>
-      </c>
-      <c r="R12" t="s">
-        <v>27</v>
+      <c r="R12">
+        <v>0</v>
       </c>
       <c r="S12" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>100</v>
       </c>
@@ -3309,28 +3427,877 @@
         <v>0.1071</v>
       </c>
       <c r="P13">
+        <f t="shared" si="0"/>
+        <v>2024.7255</v>
+      </c>
+      <c r="Q13">
         <v>2025.5356999999999</v>
       </c>
-      <c r="Q13">
-        <v>0</v>
-      </c>
-      <c r="R13" t="s">
-        <v>27</v>
+      <c r="R13">
+        <v>0</v>
       </c>
       <c r="S13" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="P14" s="10">
+        <f>SUM(P10:P13)</f>
+        <v>35662.838085000003</v>
+      </c>
+      <c r="Q14">
+        <f>SUM(Q2:Q13)</f>
+        <v>35677.108899999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="I15">
         <f>I13-J13</f>
         <v>1890.5</v>
       </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="O15">
+        <f>M10*O10</f>
+        <v>14909.348160000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="I16" s="6">
         <f>I15*E13</f>
         <v>18905</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="G17">
+        <v>6924.6</v>
+      </c>
+      <c r="H17" s="11">
+        <f>G17/1.12</f>
+        <v>6182.6785714285716</v>
+      </c>
+      <c r="K17">
+        <v>6924.6</v>
+      </c>
+      <c r="O17">
+        <f>M10/Q10</f>
+        <v>9.3333333243939762</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="H18" s="10">
+        <f>G17-H17</f>
+        <v>741.92142857142881</v>
+      </c>
+      <c r="K18">
+        <v>741.62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="K19">
+        <f>SUM(K17:K18)</f>
+        <v>7666.22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25" t="s">
+        <v>8</v>
+      </c>
+      <c r="G25" t="s">
+        <v>9</v>
+      </c>
+      <c r="H25" t="s">
+        <v>10</v>
+      </c>
+      <c r="I25" t="s">
+        <v>11</v>
+      </c>
+      <c r="J25" t="s">
+        <v>12</v>
+      </c>
+      <c r="K25" t="s">
+        <v>13</v>
+      </c>
+      <c r="L25" t="s">
+        <v>14</v>
+      </c>
+      <c r="M25" t="s">
+        <v>15</v>
+      </c>
+      <c r="N25" t="s">
+        <v>16</v>
+      </c>
+      <c r="O25" t="s">
+        <v>17</v>
+      </c>
+      <c r="P25" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>19</v>
+      </c>
+      <c r="R25" t="s">
+        <v>20</v>
+      </c>
+      <c r="S25" t="s">
+        <v>21</v>
+      </c>
+      <c r="T25" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>89</v>
+      </c>
+      <c r="B26">
+        <v>10</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>43</v>
+      </c>
+      <c r="E26">
+        <v>100</v>
+      </c>
+      <c r="F26" t="s">
+        <v>23</v>
+      </c>
+      <c r="G26" t="s">
+        <v>24</v>
+      </c>
+      <c r="H26" t="s">
+        <v>25</v>
+      </c>
+      <c r="I26">
+        <v>1633</v>
+      </c>
+      <c r="J26">
+        <v>246.37</v>
+      </c>
+      <c r="K26" t="s">
+        <v>26</v>
+      </c>
+      <c r="L26">
+        <v>1012160456169</v>
+      </c>
+      <c r="M26">
+        <v>138663</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
+      <c r="P26">
+        <v>0</v>
+      </c>
+      <c r="Q26">
+        <v>0</v>
+      </c>
+      <c r="R26" t="s">
+        <v>27</v>
+      </c>
+      <c r="S26" t="s">
+        <v>27</v>
+      </c>
+      <c r="T26">
+        <v>12345</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>90</v>
+      </c>
+      <c r="B27">
+        <v>10</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="D27">
+        <v>48</v>
+      </c>
+      <c r="E27">
+        <v>450</v>
+      </c>
+      <c r="F27" t="s">
+        <v>28</v>
+      </c>
+      <c r="G27" t="s">
+        <v>24</v>
+      </c>
+      <c r="H27" t="s">
+        <v>25</v>
+      </c>
+      <c r="I27">
+        <v>1310.75</v>
+      </c>
+      <c r="J27">
+        <v>245.35</v>
+      </c>
+      <c r="K27" t="s">
+        <v>26</v>
+      </c>
+      <c r="L27">
+        <v>1012160456171</v>
+      </c>
+      <c r="M27">
+        <v>479430</v>
+      </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
+      <c r="O27">
+        <v>0</v>
+      </c>
+      <c r="P27">
+        <v>0</v>
+      </c>
+      <c r="Q27">
+        <v>0</v>
+      </c>
+      <c r="R27" t="s">
+        <v>27</v>
+      </c>
+      <c r="S27" t="s">
+        <v>27</v>
+      </c>
+      <c r="T27">
+        <v>12345</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>91</v>
+      </c>
+      <c r="B28">
+        <v>10</v>
+      </c>
+      <c r="C28">
+        <v>3</v>
+      </c>
+      <c r="D28">
+        <v>45</v>
+      </c>
+      <c r="E28">
+        <v>300</v>
+      </c>
+      <c r="F28" t="s">
+        <v>29</v>
+      </c>
+      <c r="G28" t="s">
+        <v>24</v>
+      </c>
+      <c r="H28" t="s">
+        <v>25</v>
+      </c>
+      <c r="I28">
+        <v>1456</v>
+      </c>
+      <c r="J28">
+        <v>246.08</v>
+      </c>
+      <c r="K28" t="s">
+        <v>26</v>
+      </c>
+      <c r="L28">
+        <v>1012160456182</v>
+      </c>
+      <c r="M28">
+        <v>398976</v>
+      </c>
+      <c r="N28">
+        <v>0</v>
+      </c>
+      <c r="O28">
+        <v>0</v>
+      </c>
+      <c r="P28">
+        <v>0</v>
+      </c>
+      <c r="Q28">
+        <v>0</v>
+      </c>
+      <c r="R28" t="s">
+        <v>27</v>
+      </c>
+      <c r="S28" t="s">
+        <v>27</v>
+      </c>
+      <c r="T28">
+        <v>12344</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>92</v>
+      </c>
+      <c r="B29">
+        <v>10</v>
+      </c>
+      <c r="C29">
+        <v>4</v>
+      </c>
+      <c r="D29">
+        <v>51</v>
+      </c>
+      <c r="E29">
+        <v>50</v>
+      </c>
+      <c r="F29" t="s">
+        <v>30</v>
+      </c>
+      <c r="G29" t="s">
+        <v>24</v>
+      </c>
+      <c r="H29" t="s">
+        <v>31</v>
+      </c>
+      <c r="I29">
+        <v>737.5</v>
+      </c>
+      <c r="J29">
+        <v>123.04</v>
+      </c>
+      <c r="K29" t="s">
+        <v>26</v>
+      </c>
+      <c r="L29">
+        <v>1012160497392</v>
+      </c>
+      <c r="M29">
+        <v>30723</v>
+      </c>
+      <c r="N29">
+        <v>0</v>
+      </c>
+      <c r="O29">
+        <v>0</v>
+      </c>
+      <c r="P29">
+        <v>0</v>
+      </c>
+      <c r="Q29">
+        <v>0</v>
+      </c>
+      <c r="R29" t="s">
+        <v>27</v>
+      </c>
+      <c r="S29" t="s">
+        <v>27</v>
+      </c>
+      <c r="T29">
+        <v>12344</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>93</v>
+      </c>
+      <c r="B30">
+        <v>10</v>
+      </c>
+      <c r="C30">
+        <v>5</v>
+      </c>
+      <c r="D30">
+        <v>19</v>
+      </c>
+      <c r="E30">
+        <v>50</v>
+      </c>
+      <c r="F30" t="s">
+        <v>32</v>
+      </c>
+      <c r="G30" t="s">
+        <v>33</v>
+      </c>
+      <c r="H30" t="s">
+        <v>25</v>
+      </c>
+      <c r="I30">
+        <v>1086.75</v>
+      </c>
+      <c r="J30">
+        <v>134.78</v>
+      </c>
+      <c r="K30" t="s">
+        <v>26</v>
+      </c>
+      <c r="L30">
+        <v>1012150728560</v>
+      </c>
+      <c r="M30">
+        <v>47598.5</v>
+      </c>
+      <c r="N30">
+        <v>0</v>
+      </c>
+      <c r="O30">
+        <v>0</v>
+      </c>
+      <c r="P30">
+        <v>0</v>
+      </c>
+      <c r="Q30">
+        <v>0</v>
+      </c>
+      <c r="R30" t="s">
+        <v>27</v>
+      </c>
+      <c r="S30" t="s">
+        <v>27</v>
+      </c>
+      <c r="T30">
+        <v>12343</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>94</v>
+      </c>
+      <c r="B31">
+        <v>10</v>
+      </c>
+      <c r="C31">
+        <v>6</v>
+      </c>
+      <c r="D31">
+        <v>76</v>
+      </c>
+      <c r="E31">
+        <v>100</v>
+      </c>
+      <c r="F31" t="s">
+        <v>34</v>
+      </c>
+      <c r="G31" t="s">
+        <v>33</v>
+      </c>
+      <c r="H31" t="s">
+        <v>31</v>
+      </c>
+      <c r="I31">
+        <v>1196.5</v>
+      </c>
+      <c r="J31">
+        <v>70.66</v>
+      </c>
+      <c r="K31" t="s">
+        <v>26</v>
+      </c>
+      <c r="L31">
+        <v>1012150756003</v>
+      </c>
+      <c r="M31">
+        <v>112584</v>
+      </c>
+      <c r="N31">
+        <v>0</v>
+      </c>
+      <c r="O31">
+        <v>0</v>
+      </c>
+      <c r="P31">
+        <v>0</v>
+      </c>
+      <c r="Q31">
+        <v>0</v>
+      </c>
+      <c r="R31" t="s">
+        <v>27</v>
+      </c>
+      <c r="S31" t="s">
+        <v>27</v>
+      </c>
+      <c r="T31">
+        <v>12343</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>95</v>
+      </c>
+      <c r="B32">
+        <v>10</v>
+      </c>
+      <c r="C32">
+        <v>7</v>
+      </c>
+      <c r="D32">
+        <v>68</v>
+      </c>
+      <c r="E32">
+        <v>48</v>
+      </c>
+      <c r="F32" t="s">
+        <v>35</v>
+      </c>
+      <c r="G32" t="s">
+        <v>33</v>
+      </c>
+      <c r="H32" t="s">
+        <v>25</v>
+      </c>
+      <c r="I32">
+        <v>1441.5</v>
+      </c>
+      <c r="J32">
+        <v>136.56</v>
+      </c>
+      <c r="K32" t="s">
+        <v>26</v>
+      </c>
+      <c r="L32">
+        <v>1012150756006</v>
+      </c>
+      <c r="M32">
+        <v>62637.120000000003</v>
+      </c>
+      <c r="N32">
+        <v>0</v>
+      </c>
+      <c r="O32">
+        <v>0</v>
+      </c>
+      <c r="P32">
+        <v>0</v>
+      </c>
+      <c r="Q32">
+        <v>0</v>
+      </c>
+      <c r="R32" t="s">
+        <v>27</v>
+      </c>
+      <c r="S32" t="s">
+        <v>27</v>
+      </c>
+      <c r="T32">
+        <v>12343</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>96</v>
+      </c>
+      <c r="B33">
+        <v>10</v>
+      </c>
+      <c r="C33">
+        <v>8</v>
+      </c>
+      <c r="D33">
+        <v>41</v>
+      </c>
+      <c r="E33">
+        <v>7</v>
+      </c>
+      <c r="F33" t="s">
+        <v>36</v>
+      </c>
+      <c r="G33" t="s">
+        <v>24</v>
+      </c>
+      <c r="H33" t="s">
+        <v>25</v>
+      </c>
+      <c r="I33">
+        <v>1260</v>
+      </c>
+      <c r="J33">
+        <v>165.5</v>
+      </c>
+      <c r="K33" t="s">
+        <v>26</v>
+      </c>
+      <c r="L33">
+        <v>1012154706523</v>
+      </c>
+      <c r="M33">
+        <v>7661.5</v>
+      </c>
+      <c r="N33">
+        <v>0</v>
+      </c>
+      <c r="O33">
+        <v>0</v>
+      </c>
+      <c r="P33">
+        <v>0</v>
+      </c>
+      <c r="Q33">
+        <v>0</v>
+      </c>
+      <c r="R33" t="s">
+        <v>27</v>
+      </c>
+      <c r="S33" t="s">
+        <v>27</v>
+      </c>
+      <c r="T33">
+        <v>12343</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>97</v>
+      </c>
+      <c r="B34">
+        <v>10</v>
+      </c>
+      <c r="C34">
+        <v>9</v>
+      </c>
+      <c r="D34">
+        <v>20108</v>
+      </c>
+      <c r="E34">
+        <v>60</v>
+      </c>
+      <c r="F34" t="s">
+        <v>37</v>
+      </c>
+      <c r="G34" t="s">
+        <v>38</v>
+      </c>
+      <c r="H34" t="s">
+        <v>39</v>
+      </c>
+      <c r="I34">
+        <v>2454.5500000000002</v>
+      </c>
+      <c r="J34">
+        <v>134.38999999999999</v>
+      </c>
+      <c r="K34" t="s">
+        <v>26</v>
+      </c>
+      <c r="L34">
+        <v>1012180154191</v>
+      </c>
+      <c r="M34">
+        <v>139209.60000000001</v>
+      </c>
+      <c r="N34">
+        <v>1</v>
+      </c>
+      <c r="O34">
+        <v>0.1071</v>
+      </c>
+      <c r="P34">
+        <v>14909.3482</v>
+      </c>
+      <c r="Q34">
+        <v>0</v>
+      </c>
+      <c r="R34" t="s">
+        <v>27</v>
+      </c>
+      <c r="S34" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>98</v>
+      </c>
+      <c r="B35">
+        <v>10</v>
+      </c>
+      <c r="C35">
+        <v>10</v>
+      </c>
+      <c r="D35">
+        <v>20109</v>
+      </c>
+      <c r="E35">
+        <v>85</v>
+      </c>
+      <c r="F35" t="s">
+        <v>40</v>
+      </c>
+      <c r="G35" t="s">
+        <v>38</v>
+      </c>
+      <c r="H35" t="s">
+        <v>39</v>
+      </c>
+      <c r="I35">
+        <v>1727.27</v>
+      </c>
+      <c r="J35">
+        <v>94.56</v>
+      </c>
+      <c r="K35" t="s">
+        <v>26</v>
+      </c>
+      <c r="L35">
+        <v>1012180158558</v>
+      </c>
+      <c r="M35">
+        <v>138780.35</v>
+      </c>
+      <c r="N35">
+        <v>1</v>
+      </c>
+      <c r="O35">
+        <v>0.1071</v>
+      </c>
+      <c r="P35">
+        <v>14863.3755</v>
+      </c>
+      <c r="Q35">
+        <v>0</v>
+      </c>
+      <c r="R35" t="s">
+        <v>27</v>
+      </c>
+      <c r="S35" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>99</v>
+      </c>
+      <c r="B36">
+        <v>10</v>
+      </c>
+      <c r="C36">
+        <v>11</v>
+      </c>
+      <c r="D36">
+        <v>20110</v>
+      </c>
+      <c r="E36">
+        <v>20</v>
+      </c>
+      <c r="F36" t="s">
+        <v>41</v>
+      </c>
+      <c r="G36" t="s">
+        <v>38</v>
+      </c>
+      <c r="H36" t="s">
+        <v>39</v>
+      </c>
+      <c r="I36">
+        <v>1909.09</v>
+      </c>
+      <c r="J36">
+        <v>104.52</v>
+      </c>
+      <c r="K36" t="s">
+        <v>26</v>
+      </c>
+      <c r="L36">
+        <v>1012180154192</v>
+      </c>
+      <c r="M36">
+        <v>36091.4</v>
+      </c>
+      <c r="N36">
+        <v>1</v>
+      </c>
+      <c r="O36">
+        <v>0.1071</v>
+      </c>
+      <c r="P36">
+        <v>3865.3888999999999</v>
+      </c>
+      <c r="Q36">
+        <v>0</v>
+      </c>
+      <c r="R36" t="s">
+        <v>27</v>
+      </c>
+      <c r="S36" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>100</v>
+      </c>
+      <c r="B37">
+        <v>10</v>
+      </c>
+      <c r="C37">
+        <v>12</v>
+      </c>
+      <c r="D37">
+        <v>20111</v>
+      </c>
+      <c r="E37">
+        <v>10</v>
+      </c>
+      <c r="F37" t="s">
+        <v>42</v>
+      </c>
+      <c r="G37" t="s">
+        <v>38</v>
+      </c>
+      <c r="H37" t="s">
+        <v>39</v>
+      </c>
+      <c r="I37">
+        <v>2000</v>
+      </c>
+      <c r="J37">
+        <v>109.5</v>
+      </c>
+      <c r="K37" t="s">
+        <v>26</v>
+      </c>
+      <c r="L37">
+        <v>1012180154193</v>
+      </c>
+      <c r="M37">
+        <v>18905</v>
+      </c>
+      <c r="N37">
+        <v>1</v>
+      </c>
+      <c r="O37">
+        <v>0.1071</v>
+      </c>
+      <c r="P37">
+        <v>2024.7255</v>
+      </c>
+      <c r="Q37">
+        <v>0</v>
+      </c>
+      <c r="R37" t="s">
+        <v>27</v>
+      </c>
+      <c r="S37" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="P38">
+        <f>SUM(P26:P37)</f>
+        <v>35662.838100000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>